<commit_message>
Gaussian function fit corrected
</commit_message>
<xml_diff>
--- a/Notebooks/data/rough_samples.xlsx
+++ b/Notebooks/data/rough_samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosreyes/Desktop/Academics/postdoc/confirm/python/optosurf/Notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B788AC67-1285-2C48-8BAA-EF96C6A19C5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB60AD38-8949-524E-819B-1A35FBCC5CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44040" yWindow="1620" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{CCBD6D69-546C-D340-B48E-AE04F8667F1C}"/>
   </bookViews>
@@ -1201,7 +1201,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1323,5 +1323,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added lorentzian and tables
</commit_message>
<xml_diff>
--- a/Notebooks/data/rough_samples.xlsx
+++ b/Notebooks/data/rough_samples.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosreyes/Desktop/Academics/postdoc/confirm/python/optosurf/Notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB60AD38-8949-524E-819B-1A35FBCC5CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB71C5-D4E3-9D4C-A8D4-54653A0B26DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44040" yWindow="1620" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{CCBD6D69-546C-D340-B48E-AE04F8667F1C}"/>
+    <workbookView xWindow="43620" yWindow="2860" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{CCBD6D69-546C-D340-B48E-AE04F8667F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
-    <sheet name="Guess" sheetId="3" r:id="rId2"/>
+    <sheet name="Gaussian" sheetId="3" r:id="rId2"/>
+    <sheet name="Lorentzian" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>pt2</t>
   </si>
@@ -73,6 +74,12 @@
   </si>
   <si>
     <t>Abase</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>Alorentzian</t>
   </si>
 </sst>
 </file>
@@ -1200,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F69B1EE3-D53B-934A-A1A7-220A82AD71EA}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1254,75 +1261,205 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="C3">
-        <v>1.3</v>
+        <v>0.91</v>
       </c>
       <c r="D3">
-        <v>1.3</v>
+        <v>0.93</v>
       </c>
       <c r="E3">
-        <v>1.3</v>
+        <v>0.9</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0.82</v>
       </c>
       <c r="G3">
-        <v>1.59</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>4000</v>
+        <v>1.3</v>
       </c>
       <c r="C4">
-        <v>3250</v>
+        <v>1.3</v>
       </c>
       <c r="D4">
-        <v>2250</v>
+        <v>1.3</v>
       </c>
       <c r="E4">
-        <v>2250</v>
+        <v>1.3</v>
       </c>
       <c r="F4">
-        <v>2250</v>
+        <v>2</v>
       </c>
       <c r="G4">
-        <v>9250</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>0.9</v>
+        <v>4000</v>
       </c>
       <c r="C5">
-        <v>0.91</v>
+        <v>3250</v>
       </c>
       <c r="D5">
-        <v>0.93</v>
+        <v>2250</v>
       </c>
       <c r="E5">
-        <v>0.9</v>
+        <v>2250</v>
       </c>
       <c r="F5">
-        <v>0.82</v>
+        <v>2250</v>
       </c>
       <c r="G5">
-        <v>0.45</v>
+        <v>9250</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{260B936C-6A77-9A4D-AA50-16B3467AF53C}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.9</v>
+      </c>
+      <c r="C3">
+        <v>0.9</v>
+      </c>
+      <c r="D3">
+        <v>0.9</v>
+      </c>
+      <c r="E3">
+        <v>0.9</v>
+      </c>
+      <c r="F3">
+        <v>0.85</v>
+      </c>
+      <c r="G3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+      <c r="C4">
+        <v>0.8</v>
+      </c>
+      <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
+        <v>0.8</v>
+      </c>
+      <c r="F4">
+        <v>0.8</v>
+      </c>
+      <c r="G4">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>3500</v>
+      </c>
+      <c r="C5">
+        <v>3500</v>
+      </c>
+      <c r="D5">
+        <v>3500</v>
+      </c>
+      <c r="E5">
+        <v>3500</v>
+      </c>
+      <c r="F5">
+        <v>2000</v>
+      </c>
+      <c r="G5">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added errors between experimental and fit
</commit_message>
<xml_diff>
--- a/Notebooks/data/rough_samples.xlsx
+++ b/Notebooks/data/rough_samples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlosreyes/Desktop/Academics/postdoc/confirm/python/optosurf/Notebooks/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB71C5-D4E3-9D4C-A8D4-54653A0B26DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1045A9B9-94B4-8C40-8ECC-F37CB77E9FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43620" yWindow="2860" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{CCBD6D69-546C-D340-B48E-AE04F8667F1C}"/>
+    <workbookView xWindow="40400" yWindow="1900" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{CCBD6D69-546C-D340-B48E-AE04F8667F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -1208,7 +1208,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:H5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1279,7 +1279,7 @@
         <v>0.82</v>
       </c>
       <c r="G3">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1287,22 +1287,22 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>1.3</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1.3</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <v>1.59</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1310,22 +1310,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>4000</v>
+        <v>100</v>
       </c>
       <c r="C5">
-        <v>3250</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>2250</v>
+        <v>600</v>
       </c>
       <c r="E5">
-        <v>2250</v>
+        <v>1000</v>
       </c>
       <c r="F5">
         <v>2250</v>
       </c>
       <c r="G5">
-        <v>9250</v>
+        <v>6000</v>
       </c>
     </row>
   </sheetData>
@@ -1339,7 +1339,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:G5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,22 +1441,22 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>3500</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>3500</v>
+        <v>100</v>
       </c>
       <c r="E5">
-        <v>3500</v>
+        <v>500</v>
       </c>
       <c r="F5">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="G5">
-        <v>2000</v>
+        <v>1000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>